<commit_message>
feat: team.comagin.kr 에서만 보이는 컬럼 추가
</commit_message>
<xml_diff>
--- a/public/file/정보 대량등록 양식_v1_2023-03-03.xlsx
+++ b/public/file/정보 대량등록 양식_v1_2023-03-03.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.4575"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11700" activeTab="3"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="4294939905" windowHeight="17100"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="가맹점 등록" sheetId="1" r:id="rId4"/>
@@ -20,7 +20,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <x:si>
+    <x:t>포인트 사용여부(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>취소 여부(X)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가맹점 상호(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유저 생년월일(X)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유저 닉네임(O)</x:t>
+  </x:si>
+  <x:si>
     <x:t>유저 휴대폰번호(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>포인트 변환률(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>협력사 아이디(X)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가맹점 주소(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>가맹점 아이디(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용된 포인트(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>스탬프 사용여부(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품당 스탬프 저장개수(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>사용된 가맹점 아이디(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>상품 구매 총금액(O)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>포인트 적립 비율(O)</x:t>
   </x:si>
   <x:si>
     <x:r>
@@ -183,67 +228,22 @@
     </x:r>
   </x:si>
   <x:si>
-    <x:t>스탬프 사용여부(O)</x:t>
+    <x:t>아이디(O)</x:t>
   </x:si>
   <x:si>
-    <x:t>가맹점 아이디(O)</x:t>
+    <x:t>생년월일(X)</x:t>
   </x:si>
   <x:si>
-    <x:t>협력사 아이디(X)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>포인트 변환률(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>포인트 사용여부(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가맹점 주소(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용된 포인트(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유저 닉네임(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>취소 여부(X)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유저 생년월일(X)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>가맹점 상호(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>포인트 적립 비율(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품 구매 총금액(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>사용된 가맹점 아이디(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>상품당 스탬프 저장개수(O)</x:t>
+    <x:t>닉네임(O)</x:t>
   </x:si>
   <x:si>
     <x:t>비고(X)</x:t>
   </x:si>
   <x:si>
-    <x:t>아이디(O)</x:t>
+    <x:t>맥주소(O)</x:t>
   </x:si>
   <x:si>
     <x:t>패스워드(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>닉네임(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>맥주소(O)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>생년월일(X)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -560,7 +560,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="15">
+  <x:cellXfs count="29">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -629,6 +629,38 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
@@ -743,6 +775,96 @@
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
           <x:alignment horizontal="left" vertical="top" indent="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
@@ -1498,18 +1620,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="A1:J1"/>
+  <x:dimension ref="A1:J3"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="J1" activeCellId="0" sqref="A1:J1"/>
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="M12" activeCellId="0" sqref="M12:M12"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:cols>
-    <x:col min="1" max="1" width="17.25" customWidth="1"/>
-    <x:col min="2" max="2" width="15.375" customWidth="1"/>
-    <x:col min="3" max="3" width="22.875" customWidth="1"/>
-    <x:col min="4" max="6" width="16" customWidth="1"/>
+    <x:col min="1" max="1" width="17.25" style="20" customWidth="1"/>
+    <x:col min="2" max="2" width="15.375" style="20" customWidth="1"/>
+    <x:col min="3" max="3" width="22.875" style="20" customWidth="1"/>
+    <x:col min="4" max="6" width="16" style="6" customWidth="1"/>
     <x:col min="7" max="7" width="18.875" bestFit="1" customWidth="1"/>
     <x:col min="8" max="8" width="16.75" bestFit="1" customWidth="1"/>
     <x:col min="9" max="9" width="18.875" bestFit="1" customWidth="1"/>
@@ -1517,39 +1639,45 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:10" ht="17.149999999999999">
-      <x:c r="A1" s="1" t="s">
+      <x:c r="A1" s="21" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B1" s="22" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C1" s="22" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D1" s="7" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
-        <x:v>19</x:v>
+      <x:c r="E1" s="7" t="s">
+        <x:v>2</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
-        <x:v>20</x:v>
+      <x:c r="F1" s="7" t="s">
+        <x:v>8</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
-        <x:v>22</x:v>
+      <x:c r="G1" s="2" t="s">
+        <x:v>0</x:v>
       </x:c>
-      <x:c r="E1" s="2" t="s">
+      <x:c r="H1" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="I1" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="J1" s="3" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="F1" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="G1" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="I1" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="J1" s="3" t="s">
-        <x:v>16</x:v>
-      </x:c>
+    </x:row>
+    <x:row r="2" spans="5:5" ht="16.75">
+      <x:c r="E2" s="19"/>
+    </x:row>
+    <x:row r="3" spans="5:5" ht="16.75">
+      <x:c r="E3" s="19"/>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -1560,33 +1688,33 @@
   <x:dimension ref="A1:D1"/>
   <x:sheetViews>
     <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D1" activeCellId="0" sqref="A1:D1"/>
+      <x:selection activeCell="D42" activeCellId="0" sqref="A2:D42"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:cols>
-    <x:col min="1" max="1" width="17.25" customWidth="1"/>
-    <x:col min="2" max="2" width="18.875" customWidth="1"/>
-    <x:col min="3" max="3" width="23.875" customWidth="1"/>
+    <x:col min="1" max="1" width="17.25" style="23" customWidth="1"/>
+    <x:col min="2" max="2" width="18.875" style="23" customWidth="1"/>
+    <x:col min="3" max="3" width="23.875" style="23" customWidth="1"/>
     <x:col min="4" max="4" width="30.625" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4" ht="17.149999999999999">
-      <x:c r="A1" s="1" t="s">
-        <x:v>3</x:v>
+      <x:c r="A1" s="24" t="s">
+        <x:v>9</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
-        <x:v>4</x:v>
+      <x:c r="B1" s="25" t="s">
+        <x:v>7</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="C1" s="25" t="s">
         <x:v>21</x:v>
       </x:c>
       <x:c r="D1" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -1597,29 +1725,29 @@
   <x:dimension ref="A1:C1"/>
   <x:sheetViews>
     <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="B5" activeCellId="0" sqref="B5:B5"/>
+      <x:selection activeCell="B47" activeCellId="0" sqref="B47:B47"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:cols>
-    <x:col min="1" max="1" width="20.625" customWidth="1"/>
+    <x:col min="1" max="1" width="20.625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="22.5" customWidth="1"/>
-    <x:col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="16.375" style="8" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3" ht="17.149999999999999">
-      <x:c r="A1" s="2" t="s">
-        <x:v>0</x:v>
+      <x:c r="A1" s="7" t="s">
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B1" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>4</x:v>
       </x:c>
-      <x:c r="C1" s="3" t="s">
-        <x:v>11</x:v>
+      <x:c r="C1" s="9" t="s">
+        <x:v>3</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -1629,14 +1757,14 @@
   <x:sheetPr codeName="Sheet4"/>
   <x:dimension ref="A1:F1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D7" activeCellId="0" sqref="D7:D7"/>
+    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="A2" activeCellId="0" sqref="A2:F35"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:cols>
-    <x:col min="1" max="1" width="29.25" customWidth="1"/>
-    <x:col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="29.25" style="26" customWidth="1"/>
+    <x:col min="2" max="2" width="24" style="26" bestFit="1" customWidth="1"/>
     <x:col min="3" max="3" width="19.75" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
@@ -1644,27 +1772,27 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:6" ht="17.149999999999999">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
+      <x:c r="A1" s="27" t="s">
+        <x:v>5</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
-        <x:v>15</x:v>
+      <x:c r="B1" s="28" t="s">
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C1" s="2" t="s">
         <x:v>14</x:v>
       </x:c>
       <x:c r="D1" s="2" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E1" s="2" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="F1" s="3" t="s">
-        <x:v>10</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
@@ -1683,620 +1811,620 @@
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.399999999999999"/>
   <x:sheetData>
     <x:row r="2" spans="3:16">
-      <x:c r="C2" s="6" t="s">
-        <x:v>1</x:v>
+      <x:c r="C2" s="10" t="s">
+        <x:v>16</x:v>
       </x:c>
-      <x:c r="D2" s="7"/>
-      <x:c r="E2" s="7"/>
-      <x:c r="F2" s="7"/>
-      <x:c r="G2" s="7"/>
-      <x:c r="H2" s="7"/>
-      <x:c r="I2" s="7"/>
-      <x:c r="J2" s="7"/>
-      <x:c r="K2" s="7"/>
-      <x:c r="L2" s="7"/>
-      <x:c r="M2" s="7"/>
-      <x:c r="N2" s="7"/>
-      <x:c r="O2" s="7"/>
-      <x:c r="P2" s="8"/>
+      <x:c r="D2" s="11"/>
+      <x:c r="E2" s="11"/>
+      <x:c r="F2" s="11"/>
+      <x:c r="G2" s="11"/>
+      <x:c r="H2" s="11"/>
+      <x:c r="I2" s="11"/>
+      <x:c r="J2" s="11"/>
+      <x:c r="K2" s="11"/>
+      <x:c r="L2" s="11"/>
+      <x:c r="M2" s="11"/>
+      <x:c r="N2" s="11"/>
+      <x:c r="O2" s="11"/>
+      <x:c r="P2" s="12"/>
     </x:row>
     <x:row r="3" spans="3:16">
-      <x:c r="C3" s="9"/>
-      <x:c r="D3" s="10"/>
-      <x:c r="E3" s="10"/>
-      <x:c r="F3" s="10"/>
-      <x:c r="G3" s="10"/>
-      <x:c r="H3" s="10"/>
-      <x:c r="I3" s="10"/>
-      <x:c r="J3" s="10"/>
-      <x:c r="K3" s="10"/>
-      <x:c r="L3" s="10"/>
-      <x:c r="M3" s="10"/>
-      <x:c r="N3" s="10"/>
-      <x:c r="O3" s="10"/>
-      <x:c r="P3" s="11"/>
+      <x:c r="C3" s="13"/>
+      <x:c r="D3" s="14"/>
+      <x:c r="E3" s="14"/>
+      <x:c r="F3" s="14"/>
+      <x:c r="G3" s="14"/>
+      <x:c r="H3" s="14"/>
+      <x:c r="I3" s="14"/>
+      <x:c r="J3" s="14"/>
+      <x:c r="K3" s="14"/>
+      <x:c r="L3" s="14"/>
+      <x:c r="M3" s="14"/>
+      <x:c r="N3" s="14"/>
+      <x:c r="O3" s="14"/>
+      <x:c r="P3" s="15"/>
     </x:row>
     <x:row r="4" spans="3:16">
-      <x:c r="C4" s="9"/>
-      <x:c r="D4" s="10"/>
-      <x:c r="E4" s="10"/>
-      <x:c r="F4" s="10"/>
-      <x:c r="G4" s="10"/>
-      <x:c r="H4" s="10"/>
-      <x:c r="I4" s="10"/>
-      <x:c r="J4" s="10"/>
-      <x:c r="K4" s="10"/>
-      <x:c r="L4" s="10"/>
-      <x:c r="M4" s="10"/>
-      <x:c r="N4" s="10"/>
-      <x:c r="O4" s="10"/>
-      <x:c r="P4" s="11"/>
+      <x:c r="C4" s="13"/>
+      <x:c r="D4" s="14"/>
+      <x:c r="E4" s="14"/>
+      <x:c r="F4" s="14"/>
+      <x:c r="G4" s="14"/>
+      <x:c r="H4" s="14"/>
+      <x:c r="I4" s="14"/>
+      <x:c r="J4" s="14"/>
+      <x:c r="K4" s="14"/>
+      <x:c r="L4" s="14"/>
+      <x:c r="M4" s="14"/>
+      <x:c r="N4" s="14"/>
+      <x:c r="O4" s="14"/>
+      <x:c r="P4" s="15"/>
     </x:row>
     <x:row r="5" spans="3:16">
-      <x:c r="C5" s="9"/>
-      <x:c r="D5" s="10"/>
-      <x:c r="E5" s="10"/>
-      <x:c r="F5" s="10"/>
-      <x:c r="G5" s="10"/>
-      <x:c r="H5" s="10"/>
-      <x:c r="I5" s="10"/>
-      <x:c r="J5" s="10"/>
-      <x:c r="K5" s="10"/>
-      <x:c r="L5" s="10"/>
-      <x:c r="M5" s="10"/>
-      <x:c r="N5" s="10"/>
-      <x:c r="O5" s="10"/>
-      <x:c r="P5" s="11"/>
+      <x:c r="C5" s="13"/>
+      <x:c r="D5" s="14"/>
+      <x:c r="E5" s="14"/>
+      <x:c r="F5" s="14"/>
+      <x:c r="G5" s="14"/>
+      <x:c r="H5" s="14"/>
+      <x:c r="I5" s="14"/>
+      <x:c r="J5" s="14"/>
+      <x:c r="K5" s="14"/>
+      <x:c r="L5" s="14"/>
+      <x:c r="M5" s="14"/>
+      <x:c r="N5" s="14"/>
+      <x:c r="O5" s="14"/>
+      <x:c r="P5" s="15"/>
     </x:row>
     <x:row r="6" spans="3:16">
-      <x:c r="C6" s="9"/>
-      <x:c r="D6" s="10"/>
-      <x:c r="E6" s="10"/>
-      <x:c r="F6" s="10"/>
-      <x:c r="G6" s="10"/>
-      <x:c r="H6" s="10"/>
-      <x:c r="I6" s="10"/>
-      <x:c r="J6" s="10"/>
-      <x:c r="K6" s="10"/>
-      <x:c r="L6" s="10"/>
-      <x:c r="M6" s="10"/>
-      <x:c r="N6" s="10"/>
-      <x:c r="O6" s="10"/>
-      <x:c r="P6" s="11"/>
+      <x:c r="C6" s="13"/>
+      <x:c r="D6" s="14"/>
+      <x:c r="E6" s="14"/>
+      <x:c r="F6" s="14"/>
+      <x:c r="G6" s="14"/>
+      <x:c r="H6" s="14"/>
+      <x:c r="I6" s="14"/>
+      <x:c r="J6" s="14"/>
+      <x:c r="K6" s="14"/>
+      <x:c r="L6" s="14"/>
+      <x:c r="M6" s="14"/>
+      <x:c r="N6" s="14"/>
+      <x:c r="O6" s="14"/>
+      <x:c r="P6" s="15"/>
     </x:row>
     <x:row r="7" spans="3:16">
-      <x:c r="C7" s="9"/>
-      <x:c r="D7" s="10"/>
-      <x:c r="E7" s="10"/>
-      <x:c r="F7" s="10"/>
-      <x:c r="G7" s="10"/>
-      <x:c r="H7" s="10"/>
-      <x:c r="I7" s="10"/>
-      <x:c r="J7" s="10"/>
-      <x:c r="K7" s="10"/>
-      <x:c r="L7" s="10"/>
-      <x:c r="M7" s="10"/>
-      <x:c r="N7" s="10"/>
-      <x:c r="O7" s="10"/>
-      <x:c r="P7" s="11"/>
+      <x:c r="C7" s="13"/>
+      <x:c r="D7" s="14"/>
+      <x:c r="E7" s="14"/>
+      <x:c r="F7" s="14"/>
+      <x:c r="G7" s="14"/>
+      <x:c r="H7" s="14"/>
+      <x:c r="I7" s="14"/>
+      <x:c r="J7" s="14"/>
+      <x:c r="K7" s="14"/>
+      <x:c r="L7" s="14"/>
+      <x:c r="M7" s="14"/>
+      <x:c r="N7" s="14"/>
+      <x:c r="O7" s="14"/>
+      <x:c r="P7" s="15"/>
     </x:row>
     <x:row r="8" spans="3:16">
-      <x:c r="C8" s="9"/>
-      <x:c r="D8" s="10"/>
-      <x:c r="E8" s="10"/>
-      <x:c r="F8" s="10"/>
-      <x:c r="G8" s="10"/>
-      <x:c r="H8" s="10"/>
-      <x:c r="I8" s="10"/>
-      <x:c r="J8" s="10"/>
-      <x:c r="K8" s="10"/>
-      <x:c r="L8" s="10"/>
-      <x:c r="M8" s="10"/>
-      <x:c r="N8" s="10"/>
-      <x:c r="O8" s="10"/>
-      <x:c r="P8" s="11"/>
+      <x:c r="C8" s="13"/>
+      <x:c r="D8" s="14"/>
+      <x:c r="E8" s="14"/>
+      <x:c r="F8" s="14"/>
+      <x:c r="G8" s="14"/>
+      <x:c r="H8" s="14"/>
+      <x:c r="I8" s="14"/>
+      <x:c r="J8" s="14"/>
+      <x:c r="K8" s="14"/>
+      <x:c r="L8" s="14"/>
+      <x:c r="M8" s="14"/>
+      <x:c r="N8" s="14"/>
+      <x:c r="O8" s="14"/>
+      <x:c r="P8" s="15"/>
     </x:row>
     <x:row r="9" spans="3:16">
-      <x:c r="C9" s="9"/>
-      <x:c r="D9" s="10"/>
-      <x:c r="E9" s="10"/>
-      <x:c r="F9" s="10"/>
-      <x:c r="G9" s="10"/>
-      <x:c r="H9" s="10"/>
-      <x:c r="I9" s="10"/>
-      <x:c r="J9" s="10"/>
-      <x:c r="K9" s="10"/>
-      <x:c r="L9" s="10"/>
-      <x:c r="M9" s="10"/>
-      <x:c r="N9" s="10"/>
-      <x:c r="O9" s="10"/>
-      <x:c r="P9" s="11"/>
+      <x:c r="C9" s="13"/>
+      <x:c r="D9" s="14"/>
+      <x:c r="E9" s="14"/>
+      <x:c r="F9" s="14"/>
+      <x:c r="G9" s="14"/>
+      <x:c r="H9" s="14"/>
+      <x:c r="I9" s="14"/>
+      <x:c r="J9" s="14"/>
+      <x:c r="K9" s="14"/>
+      <x:c r="L9" s="14"/>
+      <x:c r="M9" s="14"/>
+      <x:c r="N9" s="14"/>
+      <x:c r="O9" s="14"/>
+      <x:c r="P9" s="15"/>
     </x:row>
     <x:row r="10" spans="3:16">
-      <x:c r="C10" s="9"/>
-      <x:c r="D10" s="10"/>
-      <x:c r="E10" s="10"/>
-      <x:c r="F10" s="10"/>
-      <x:c r="G10" s="10"/>
-      <x:c r="H10" s="10"/>
-      <x:c r="I10" s="10"/>
-      <x:c r="J10" s="10"/>
-      <x:c r="K10" s="10"/>
-      <x:c r="L10" s="10"/>
-      <x:c r="M10" s="10"/>
-      <x:c r="N10" s="10"/>
-      <x:c r="O10" s="10"/>
-      <x:c r="P10" s="11"/>
+      <x:c r="C10" s="13"/>
+      <x:c r="D10" s="14"/>
+      <x:c r="E10" s="14"/>
+      <x:c r="F10" s="14"/>
+      <x:c r="G10" s="14"/>
+      <x:c r="H10" s="14"/>
+      <x:c r="I10" s="14"/>
+      <x:c r="J10" s="14"/>
+      <x:c r="K10" s="14"/>
+      <x:c r="L10" s="14"/>
+      <x:c r="M10" s="14"/>
+      <x:c r="N10" s="14"/>
+      <x:c r="O10" s="14"/>
+      <x:c r="P10" s="15"/>
     </x:row>
     <x:row r="11" spans="3:16">
-      <x:c r="C11" s="9"/>
-      <x:c r="D11" s="10"/>
-      <x:c r="E11" s="10"/>
-      <x:c r="F11" s="10"/>
-      <x:c r="G11" s="10"/>
-      <x:c r="H11" s="10"/>
-      <x:c r="I11" s="10"/>
-      <x:c r="J11" s="10"/>
-      <x:c r="K11" s="10"/>
-      <x:c r="L11" s="10"/>
-      <x:c r="M11" s="10"/>
-      <x:c r="N11" s="10"/>
-      <x:c r="O11" s="10"/>
-      <x:c r="P11" s="11"/>
+      <x:c r="C11" s="13"/>
+      <x:c r="D11" s="14"/>
+      <x:c r="E11" s="14"/>
+      <x:c r="F11" s="14"/>
+      <x:c r="G11" s="14"/>
+      <x:c r="H11" s="14"/>
+      <x:c r="I11" s="14"/>
+      <x:c r="J11" s="14"/>
+      <x:c r="K11" s="14"/>
+      <x:c r="L11" s="14"/>
+      <x:c r="M11" s="14"/>
+      <x:c r="N11" s="14"/>
+      <x:c r="O11" s="14"/>
+      <x:c r="P11" s="15"/>
     </x:row>
     <x:row r="12" spans="3:16">
-      <x:c r="C12" s="9"/>
-      <x:c r="D12" s="10"/>
-      <x:c r="E12" s="10"/>
-      <x:c r="F12" s="10"/>
-      <x:c r="G12" s="10"/>
-      <x:c r="H12" s="10"/>
-      <x:c r="I12" s="10"/>
-      <x:c r="J12" s="10"/>
-      <x:c r="K12" s="10"/>
-      <x:c r="L12" s="10"/>
-      <x:c r="M12" s="10"/>
-      <x:c r="N12" s="10"/>
-      <x:c r="O12" s="10"/>
-      <x:c r="P12" s="11"/>
+      <x:c r="C12" s="13"/>
+      <x:c r="D12" s="14"/>
+      <x:c r="E12" s="14"/>
+      <x:c r="F12" s="14"/>
+      <x:c r="G12" s="14"/>
+      <x:c r="H12" s="14"/>
+      <x:c r="I12" s="14"/>
+      <x:c r="J12" s="14"/>
+      <x:c r="K12" s="14"/>
+      <x:c r="L12" s="14"/>
+      <x:c r="M12" s="14"/>
+      <x:c r="N12" s="14"/>
+      <x:c r="O12" s="14"/>
+      <x:c r="P12" s="15"/>
     </x:row>
     <x:row r="13" spans="3:16">
-      <x:c r="C13" s="9"/>
-      <x:c r="D13" s="10"/>
-      <x:c r="E13" s="10"/>
-      <x:c r="F13" s="10"/>
-      <x:c r="G13" s="10"/>
-      <x:c r="H13" s="10"/>
-      <x:c r="I13" s="10"/>
-      <x:c r="J13" s="10"/>
-      <x:c r="K13" s="10"/>
-      <x:c r="L13" s="10"/>
-      <x:c r="M13" s="10"/>
-      <x:c r="N13" s="10"/>
-      <x:c r="O13" s="10"/>
-      <x:c r="P13" s="11"/>
+      <x:c r="C13" s="13"/>
+      <x:c r="D13" s="14"/>
+      <x:c r="E13" s="14"/>
+      <x:c r="F13" s="14"/>
+      <x:c r="G13" s="14"/>
+      <x:c r="H13" s="14"/>
+      <x:c r="I13" s="14"/>
+      <x:c r="J13" s="14"/>
+      <x:c r="K13" s="14"/>
+      <x:c r="L13" s="14"/>
+      <x:c r="M13" s="14"/>
+      <x:c r="N13" s="14"/>
+      <x:c r="O13" s="14"/>
+      <x:c r="P13" s="15"/>
     </x:row>
     <x:row r="14" spans="3:16">
-      <x:c r="C14" s="9"/>
-      <x:c r="D14" s="10"/>
-      <x:c r="E14" s="10"/>
-      <x:c r="F14" s="10"/>
-      <x:c r="G14" s="10"/>
-      <x:c r="H14" s="10"/>
-      <x:c r="I14" s="10"/>
-      <x:c r="J14" s="10"/>
-      <x:c r="K14" s="10"/>
-      <x:c r="L14" s="10"/>
-      <x:c r="M14" s="10"/>
-      <x:c r="N14" s="10"/>
-      <x:c r="O14" s="10"/>
-      <x:c r="P14" s="11"/>
+      <x:c r="C14" s="13"/>
+      <x:c r="D14" s="14"/>
+      <x:c r="E14" s="14"/>
+      <x:c r="F14" s="14"/>
+      <x:c r="G14" s="14"/>
+      <x:c r="H14" s="14"/>
+      <x:c r="I14" s="14"/>
+      <x:c r="J14" s="14"/>
+      <x:c r="K14" s="14"/>
+      <x:c r="L14" s="14"/>
+      <x:c r="M14" s="14"/>
+      <x:c r="N14" s="14"/>
+      <x:c r="O14" s="14"/>
+      <x:c r="P14" s="15"/>
     </x:row>
     <x:row r="15" spans="3:16">
-      <x:c r="C15" s="9"/>
-      <x:c r="D15" s="10"/>
-      <x:c r="E15" s="10"/>
-      <x:c r="F15" s="10"/>
-      <x:c r="G15" s="10"/>
-      <x:c r="H15" s="10"/>
-      <x:c r="I15" s="10"/>
-      <x:c r="J15" s="10"/>
-      <x:c r="K15" s="10"/>
-      <x:c r="L15" s="10"/>
-      <x:c r="M15" s="10"/>
-      <x:c r="N15" s="10"/>
-      <x:c r="O15" s="10"/>
-      <x:c r="P15" s="11"/>
+      <x:c r="C15" s="13"/>
+      <x:c r="D15" s="14"/>
+      <x:c r="E15" s="14"/>
+      <x:c r="F15" s="14"/>
+      <x:c r="G15" s="14"/>
+      <x:c r="H15" s="14"/>
+      <x:c r="I15" s="14"/>
+      <x:c r="J15" s="14"/>
+      <x:c r="K15" s="14"/>
+      <x:c r="L15" s="14"/>
+      <x:c r="M15" s="14"/>
+      <x:c r="N15" s="14"/>
+      <x:c r="O15" s="14"/>
+      <x:c r="P15" s="15"/>
     </x:row>
     <x:row r="16" spans="3:16">
-      <x:c r="C16" s="9"/>
-      <x:c r="D16" s="10"/>
-      <x:c r="E16" s="10"/>
-      <x:c r="F16" s="10"/>
-      <x:c r="G16" s="10"/>
-      <x:c r="H16" s="10"/>
-      <x:c r="I16" s="10"/>
-      <x:c r="J16" s="10"/>
-      <x:c r="K16" s="10"/>
-      <x:c r="L16" s="10"/>
-      <x:c r="M16" s="10"/>
-      <x:c r="N16" s="10"/>
-      <x:c r="O16" s="10"/>
-      <x:c r="P16" s="11"/>
+      <x:c r="C16" s="13"/>
+      <x:c r="D16" s="14"/>
+      <x:c r="E16" s="14"/>
+      <x:c r="F16" s="14"/>
+      <x:c r="G16" s="14"/>
+      <x:c r="H16" s="14"/>
+      <x:c r="I16" s="14"/>
+      <x:c r="J16" s="14"/>
+      <x:c r="K16" s="14"/>
+      <x:c r="L16" s="14"/>
+      <x:c r="M16" s="14"/>
+      <x:c r="N16" s="14"/>
+      <x:c r="O16" s="14"/>
+      <x:c r="P16" s="15"/>
     </x:row>
     <x:row r="17" spans="3:16">
-      <x:c r="C17" s="9"/>
-      <x:c r="D17" s="10"/>
-      <x:c r="E17" s="10"/>
-      <x:c r="F17" s="10"/>
-      <x:c r="G17" s="10"/>
-      <x:c r="H17" s="10"/>
-      <x:c r="I17" s="10"/>
-      <x:c r="J17" s="10"/>
-      <x:c r="K17" s="10"/>
-      <x:c r="L17" s="10"/>
-      <x:c r="M17" s="10"/>
-      <x:c r="N17" s="10"/>
-      <x:c r="O17" s="10"/>
-      <x:c r="P17" s="11"/>
+      <x:c r="C17" s="13"/>
+      <x:c r="D17" s="14"/>
+      <x:c r="E17" s="14"/>
+      <x:c r="F17" s="14"/>
+      <x:c r="G17" s="14"/>
+      <x:c r="H17" s="14"/>
+      <x:c r="I17" s="14"/>
+      <x:c r="J17" s="14"/>
+      <x:c r="K17" s="14"/>
+      <x:c r="L17" s="14"/>
+      <x:c r="M17" s="14"/>
+      <x:c r="N17" s="14"/>
+      <x:c r="O17" s="14"/>
+      <x:c r="P17" s="15"/>
     </x:row>
     <x:row r="18" spans="3:16">
-      <x:c r="C18" s="9"/>
-      <x:c r="D18" s="10"/>
-      <x:c r="E18" s="10"/>
-      <x:c r="F18" s="10"/>
-      <x:c r="G18" s="10"/>
-      <x:c r="H18" s="10"/>
-      <x:c r="I18" s="10"/>
-      <x:c r="J18" s="10"/>
-      <x:c r="K18" s="10"/>
-      <x:c r="L18" s="10"/>
-      <x:c r="M18" s="10"/>
-      <x:c r="N18" s="10"/>
-      <x:c r="O18" s="10"/>
-      <x:c r="P18" s="11"/>
+      <x:c r="C18" s="13"/>
+      <x:c r="D18" s="14"/>
+      <x:c r="E18" s="14"/>
+      <x:c r="F18" s="14"/>
+      <x:c r="G18" s="14"/>
+      <x:c r="H18" s="14"/>
+      <x:c r="I18" s="14"/>
+      <x:c r="J18" s="14"/>
+      <x:c r="K18" s="14"/>
+      <x:c r="L18" s="14"/>
+      <x:c r="M18" s="14"/>
+      <x:c r="N18" s="14"/>
+      <x:c r="O18" s="14"/>
+      <x:c r="P18" s="15"/>
     </x:row>
     <x:row r="19" spans="3:16">
-      <x:c r="C19" s="9"/>
-      <x:c r="D19" s="10"/>
-      <x:c r="E19" s="10"/>
-      <x:c r="F19" s="10"/>
-      <x:c r="G19" s="10"/>
-      <x:c r="H19" s="10"/>
-      <x:c r="I19" s="10"/>
-      <x:c r="J19" s="10"/>
-      <x:c r="K19" s="10"/>
-      <x:c r="L19" s="10"/>
-      <x:c r="M19" s="10"/>
-      <x:c r="N19" s="10"/>
-      <x:c r="O19" s="10"/>
-      <x:c r="P19" s="11"/>
+      <x:c r="C19" s="13"/>
+      <x:c r="D19" s="14"/>
+      <x:c r="E19" s="14"/>
+      <x:c r="F19" s="14"/>
+      <x:c r="G19" s="14"/>
+      <x:c r="H19" s="14"/>
+      <x:c r="I19" s="14"/>
+      <x:c r="J19" s="14"/>
+      <x:c r="K19" s="14"/>
+      <x:c r="L19" s="14"/>
+      <x:c r="M19" s="14"/>
+      <x:c r="N19" s="14"/>
+      <x:c r="O19" s="14"/>
+      <x:c r="P19" s="15"/>
     </x:row>
     <x:row r="20" spans="3:16">
-      <x:c r="C20" s="9"/>
-      <x:c r="D20" s="10"/>
-      <x:c r="E20" s="10"/>
-      <x:c r="F20" s="10"/>
-      <x:c r="G20" s="10"/>
-      <x:c r="H20" s="10"/>
-      <x:c r="I20" s="10"/>
-      <x:c r="J20" s="10"/>
-      <x:c r="K20" s="10"/>
-      <x:c r="L20" s="10"/>
-      <x:c r="M20" s="10"/>
-      <x:c r="N20" s="10"/>
-      <x:c r="O20" s="10"/>
-      <x:c r="P20" s="11"/>
+      <x:c r="C20" s="13"/>
+      <x:c r="D20" s="14"/>
+      <x:c r="E20" s="14"/>
+      <x:c r="F20" s="14"/>
+      <x:c r="G20" s="14"/>
+      <x:c r="H20" s="14"/>
+      <x:c r="I20" s="14"/>
+      <x:c r="J20" s="14"/>
+      <x:c r="K20" s="14"/>
+      <x:c r="L20" s="14"/>
+      <x:c r="M20" s="14"/>
+      <x:c r="N20" s="14"/>
+      <x:c r="O20" s="14"/>
+      <x:c r="P20" s="15"/>
     </x:row>
     <x:row r="21" spans="3:16">
-      <x:c r="C21" s="9"/>
-      <x:c r="D21" s="10"/>
-      <x:c r="E21" s="10"/>
-      <x:c r="F21" s="10"/>
-      <x:c r="G21" s="10"/>
-      <x:c r="H21" s="10"/>
-      <x:c r="I21" s="10"/>
-      <x:c r="J21" s="10"/>
-      <x:c r="K21" s="10"/>
-      <x:c r="L21" s="10"/>
-      <x:c r="M21" s="10"/>
-      <x:c r="N21" s="10"/>
-      <x:c r="O21" s="10"/>
-      <x:c r="P21" s="11"/>
+      <x:c r="C21" s="13"/>
+      <x:c r="D21" s="14"/>
+      <x:c r="E21" s="14"/>
+      <x:c r="F21" s="14"/>
+      <x:c r="G21" s="14"/>
+      <x:c r="H21" s="14"/>
+      <x:c r="I21" s="14"/>
+      <x:c r="J21" s="14"/>
+      <x:c r="K21" s="14"/>
+      <x:c r="L21" s="14"/>
+      <x:c r="M21" s="14"/>
+      <x:c r="N21" s="14"/>
+      <x:c r="O21" s="14"/>
+      <x:c r="P21" s="15"/>
     </x:row>
     <x:row r="22" spans="3:16">
-      <x:c r="C22" s="9"/>
-      <x:c r="D22" s="10"/>
-      <x:c r="E22" s="10"/>
-      <x:c r="F22" s="10"/>
-      <x:c r="G22" s="10"/>
-      <x:c r="H22" s="10"/>
-      <x:c r="I22" s="10"/>
-      <x:c r="J22" s="10"/>
-      <x:c r="K22" s="10"/>
-      <x:c r="L22" s="10"/>
-      <x:c r="M22" s="10"/>
-      <x:c r="N22" s="10"/>
-      <x:c r="O22" s="10"/>
-      <x:c r="P22" s="11"/>
+      <x:c r="C22" s="13"/>
+      <x:c r="D22" s="14"/>
+      <x:c r="E22" s="14"/>
+      <x:c r="F22" s="14"/>
+      <x:c r="G22" s="14"/>
+      <x:c r="H22" s="14"/>
+      <x:c r="I22" s="14"/>
+      <x:c r="J22" s="14"/>
+      <x:c r="K22" s="14"/>
+      <x:c r="L22" s="14"/>
+      <x:c r="M22" s="14"/>
+      <x:c r="N22" s="14"/>
+      <x:c r="O22" s="14"/>
+      <x:c r="P22" s="15"/>
     </x:row>
     <x:row r="23" spans="3:16">
-      <x:c r="C23" s="9"/>
-      <x:c r="D23" s="10"/>
-      <x:c r="E23" s="10"/>
-      <x:c r="F23" s="10"/>
-      <x:c r="G23" s="10"/>
-      <x:c r="H23" s="10"/>
-      <x:c r="I23" s="10"/>
-      <x:c r="J23" s="10"/>
-      <x:c r="K23" s="10"/>
-      <x:c r="L23" s="10"/>
-      <x:c r="M23" s="10"/>
-      <x:c r="N23" s="10"/>
-      <x:c r="O23" s="10"/>
-      <x:c r="P23" s="11"/>
+      <x:c r="C23" s="13"/>
+      <x:c r="D23" s="14"/>
+      <x:c r="E23" s="14"/>
+      <x:c r="F23" s="14"/>
+      <x:c r="G23" s="14"/>
+      <x:c r="H23" s="14"/>
+      <x:c r="I23" s="14"/>
+      <x:c r="J23" s="14"/>
+      <x:c r="K23" s="14"/>
+      <x:c r="L23" s="14"/>
+      <x:c r="M23" s="14"/>
+      <x:c r="N23" s="14"/>
+      <x:c r="O23" s="14"/>
+      <x:c r="P23" s="15"/>
     </x:row>
     <x:row r="24" spans="3:16">
-      <x:c r="C24" s="9"/>
-      <x:c r="D24" s="10"/>
-      <x:c r="E24" s="10"/>
-      <x:c r="F24" s="10"/>
-      <x:c r="G24" s="10"/>
-      <x:c r="H24" s="10"/>
-      <x:c r="I24" s="10"/>
-      <x:c r="J24" s="10"/>
-      <x:c r="K24" s="10"/>
-      <x:c r="L24" s="10"/>
-      <x:c r="M24" s="10"/>
-      <x:c r="N24" s="10"/>
-      <x:c r="O24" s="10"/>
-      <x:c r="P24" s="11"/>
+      <x:c r="C24" s="13"/>
+      <x:c r="D24" s="14"/>
+      <x:c r="E24" s="14"/>
+      <x:c r="F24" s="14"/>
+      <x:c r="G24" s="14"/>
+      <x:c r="H24" s="14"/>
+      <x:c r="I24" s="14"/>
+      <x:c r="J24" s="14"/>
+      <x:c r="K24" s="14"/>
+      <x:c r="L24" s="14"/>
+      <x:c r="M24" s="14"/>
+      <x:c r="N24" s="14"/>
+      <x:c r="O24" s="14"/>
+      <x:c r="P24" s="15"/>
     </x:row>
     <x:row r="25" spans="3:16">
-      <x:c r="C25" s="9"/>
-      <x:c r="D25" s="10"/>
-      <x:c r="E25" s="10"/>
-      <x:c r="F25" s="10"/>
-      <x:c r="G25" s="10"/>
-      <x:c r="H25" s="10"/>
-      <x:c r="I25" s="10"/>
-      <x:c r="J25" s="10"/>
-      <x:c r="K25" s="10"/>
-      <x:c r="L25" s="10"/>
-      <x:c r="M25" s="10"/>
-      <x:c r="N25" s="10"/>
-      <x:c r="O25" s="10"/>
-      <x:c r="P25" s="11"/>
+      <x:c r="C25" s="13"/>
+      <x:c r="D25" s="14"/>
+      <x:c r="E25" s="14"/>
+      <x:c r="F25" s="14"/>
+      <x:c r="G25" s="14"/>
+      <x:c r="H25" s="14"/>
+      <x:c r="I25" s="14"/>
+      <x:c r="J25" s="14"/>
+      <x:c r="K25" s="14"/>
+      <x:c r="L25" s="14"/>
+      <x:c r="M25" s="14"/>
+      <x:c r="N25" s="14"/>
+      <x:c r="O25" s="14"/>
+      <x:c r="P25" s="15"/>
     </x:row>
     <x:row r="26" spans="3:16">
-      <x:c r="C26" s="9"/>
-      <x:c r="D26" s="10"/>
-      <x:c r="E26" s="10"/>
-      <x:c r="F26" s="10"/>
-      <x:c r="G26" s="10"/>
-      <x:c r="H26" s="10"/>
-      <x:c r="I26" s="10"/>
-      <x:c r="J26" s="10"/>
-      <x:c r="K26" s="10"/>
-      <x:c r="L26" s="10"/>
-      <x:c r="M26" s="10"/>
-      <x:c r="N26" s="10"/>
-      <x:c r="O26" s="10"/>
-      <x:c r="P26" s="11"/>
+      <x:c r="C26" s="13"/>
+      <x:c r="D26" s="14"/>
+      <x:c r="E26" s="14"/>
+      <x:c r="F26" s="14"/>
+      <x:c r="G26" s="14"/>
+      <x:c r="H26" s="14"/>
+      <x:c r="I26" s="14"/>
+      <x:c r="J26" s="14"/>
+      <x:c r="K26" s="14"/>
+      <x:c r="L26" s="14"/>
+      <x:c r="M26" s="14"/>
+      <x:c r="N26" s="14"/>
+      <x:c r="O26" s="14"/>
+      <x:c r="P26" s="15"/>
     </x:row>
     <x:row r="27" spans="3:16">
-      <x:c r="C27" s="9"/>
-      <x:c r="D27" s="10"/>
-      <x:c r="E27" s="10"/>
-      <x:c r="F27" s="10"/>
-      <x:c r="G27" s="10"/>
-      <x:c r="H27" s="10"/>
-      <x:c r="I27" s="10"/>
-      <x:c r="J27" s="10"/>
-      <x:c r="K27" s="10"/>
-      <x:c r="L27" s="10"/>
-      <x:c r="M27" s="10"/>
-      <x:c r="N27" s="10"/>
-      <x:c r="O27" s="10"/>
-      <x:c r="P27" s="11"/>
+      <x:c r="C27" s="13"/>
+      <x:c r="D27" s="14"/>
+      <x:c r="E27" s="14"/>
+      <x:c r="F27" s="14"/>
+      <x:c r="G27" s="14"/>
+      <x:c r="H27" s="14"/>
+      <x:c r="I27" s="14"/>
+      <x:c r="J27" s="14"/>
+      <x:c r="K27" s="14"/>
+      <x:c r="L27" s="14"/>
+      <x:c r="M27" s="14"/>
+      <x:c r="N27" s="14"/>
+      <x:c r="O27" s="14"/>
+      <x:c r="P27" s="15"/>
     </x:row>
     <x:row r="28" spans="3:16">
-      <x:c r="C28" s="9"/>
-      <x:c r="D28" s="10"/>
-      <x:c r="E28" s="10"/>
-      <x:c r="F28" s="10"/>
-      <x:c r="G28" s="10"/>
-      <x:c r="H28" s="10"/>
-      <x:c r="I28" s="10"/>
-      <x:c r="J28" s="10"/>
-      <x:c r="K28" s="10"/>
-      <x:c r="L28" s="10"/>
-      <x:c r="M28" s="10"/>
-      <x:c r="N28" s="10"/>
-      <x:c r="O28" s="10"/>
-      <x:c r="P28" s="11"/>
+      <x:c r="C28" s="13"/>
+      <x:c r="D28" s="14"/>
+      <x:c r="E28" s="14"/>
+      <x:c r="F28" s="14"/>
+      <x:c r="G28" s="14"/>
+      <x:c r="H28" s="14"/>
+      <x:c r="I28" s="14"/>
+      <x:c r="J28" s="14"/>
+      <x:c r="K28" s="14"/>
+      <x:c r="L28" s="14"/>
+      <x:c r="M28" s="14"/>
+      <x:c r="N28" s="14"/>
+      <x:c r="O28" s="14"/>
+      <x:c r="P28" s="15"/>
     </x:row>
     <x:row r="29" spans="3:16">
-      <x:c r="C29" s="9"/>
-      <x:c r="D29" s="10"/>
-      <x:c r="E29" s="10"/>
-      <x:c r="F29" s="10"/>
-      <x:c r="G29" s="10"/>
-      <x:c r="H29" s="10"/>
-      <x:c r="I29" s="10"/>
-      <x:c r="J29" s="10"/>
-      <x:c r="K29" s="10"/>
-      <x:c r="L29" s="10"/>
-      <x:c r="M29" s="10"/>
-      <x:c r="N29" s="10"/>
-      <x:c r="O29" s="10"/>
-      <x:c r="P29" s="11"/>
+      <x:c r="C29" s="13"/>
+      <x:c r="D29" s="14"/>
+      <x:c r="E29" s="14"/>
+      <x:c r="F29" s="14"/>
+      <x:c r="G29" s="14"/>
+      <x:c r="H29" s="14"/>
+      <x:c r="I29" s="14"/>
+      <x:c r="J29" s="14"/>
+      <x:c r="K29" s="14"/>
+      <x:c r="L29" s="14"/>
+      <x:c r="M29" s="14"/>
+      <x:c r="N29" s="14"/>
+      <x:c r="O29" s="14"/>
+      <x:c r="P29" s="15"/>
     </x:row>
     <x:row r="30" spans="3:16">
-      <x:c r="C30" s="9"/>
-      <x:c r="D30" s="10"/>
-      <x:c r="E30" s="10"/>
-      <x:c r="F30" s="10"/>
-      <x:c r="G30" s="10"/>
-      <x:c r="H30" s="10"/>
-      <x:c r="I30" s="10"/>
-      <x:c r="J30" s="10"/>
-      <x:c r="K30" s="10"/>
-      <x:c r="L30" s="10"/>
-      <x:c r="M30" s="10"/>
-      <x:c r="N30" s="10"/>
-      <x:c r="O30" s="10"/>
-      <x:c r="P30" s="11"/>
+      <x:c r="C30" s="13"/>
+      <x:c r="D30" s="14"/>
+      <x:c r="E30" s="14"/>
+      <x:c r="F30" s="14"/>
+      <x:c r="G30" s="14"/>
+      <x:c r="H30" s="14"/>
+      <x:c r="I30" s="14"/>
+      <x:c r="J30" s="14"/>
+      <x:c r="K30" s="14"/>
+      <x:c r="L30" s="14"/>
+      <x:c r="M30" s="14"/>
+      <x:c r="N30" s="14"/>
+      <x:c r="O30" s="14"/>
+      <x:c r="P30" s="15"/>
     </x:row>
     <x:row r="31" spans="3:16">
-      <x:c r="C31" s="9"/>
-      <x:c r="D31" s="10"/>
-      <x:c r="E31" s="10"/>
-      <x:c r="F31" s="10"/>
-      <x:c r="G31" s="10"/>
-      <x:c r="H31" s="10"/>
-      <x:c r="I31" s="10"/>
-      <x:c r="J31" s="10"/>
-      <x:c r="K31" s="10"/>
-      <x:c r="L31" s="10"/>
-      <x:c r="M31" s="10"/>
-      <x:c r="N31" s="10"/>
-      <x:c r="O31" s="10"/>
-      <x:c r="P31" s="11"/>
+      <x:c r="C31" s="13"/>
+      <x:c r="D31" s="14"/>
+      <x:c r="E31" s="14"/>
+      <x:c r="F31" s="14"/>
+      <x:c r="G31" s="14"/>
+      <x:c r="H31" s="14"/>
+      <x:c r="I31" s="14"/>
+      <x:c r="J31" s="14"/>
+      <x:c r="K31" s="14"/>
+      <x:c r="L31" s="14"/>
+      <x:c r="M31" s="14"/>
+      <x:c r="N31" s="14"/>
+      <x:c r="O31" s="14"/>
+      <x:c r="P31" s="15"/>
     </x:row>
     <x:row r="32" spans="3:16">
-      <x:c r="C32" s="9"/>
-      <x:c r="D32" s="10"/>
-      <x:c r="E32" s="10"/>
-      <x:c r="F32" s="10"/>
-      <x:c r="G32" s="10"/>
-      <x:c r="H32" s="10"/>
-      <x:c r="I32" s="10"/>
-      <x:c r="J32" s="10"/>
-      <x:c r="K32" s="10"/>
-      <x:c r="L32" s="10"/>
-      <x:c r="M32" s="10"/>
-      <x:c r="N32" s="10"/>
-      <x:c r="O32" s="10"/>
-      <x:c r="P32" s="11"/>
+      <x:c r="C32" s="13"/>
+      <x:c r="D32" s="14"/>
+      <x:c r="E32" s="14"/>
+      <x:c r="F32" s="14"/>
+      <x:c r="G32" s="14"/>
+      <x:c r="H32" s="14"/>
+      <x:c r="I32" s="14"/>
+      <x:c r="J32" s="14"/>
+      <x:c r="K32" s="14"/>
+      <x:c r="L32" s="14"/>
+      <x:c r="M32" s="14"/>
+      <x:c r="N32" s="14"/>
+      <x:c r="O32" s="14"/>
+      <x:c r="P32" s="15"/>
     </x:row>
     <x:row r="33" spans="3:16">
-      <x:c r="C33" s="9"/>
-      <x:c r="D33" s="10"/>
-      <x:c r="E33" s="10"/>
-      <x:c r="F33" s="10"/>
-      <x:c r="G33" s="10"/>
-      <x:c r="H33" s="10"/>
-      <x:c r="I33" s="10"/>
-      <x:c r="J33" s="10"/>
-      <x:c r="K33" s="10"/>
-      <x:c r="L33" s="10"/>
-      <x:c r="M33" s="10"/>
-      <x:c r="N33" s="10"/>
-      <x:c r="O33" s="10"/>
-      <x:c r="P33" s="11"/>
+      <x:c r="C33" s="13"/>
+      <x:c r="D33" s="14"/>
+      <x:c r="E33" s="14"/>
+      <x:c r="F33" s="14"/>
+      <x:c r="G33" s="14"/>
+      <x:c r="H33" s="14"/>
+      <x:c r="I33" s="14"/>
+      <x:c r="J33" s="14"/>
+      <x:c r="K33" s="14"/>
+      <x:c r="L33" s="14"/>
+      <x:c r="M33" s="14"/>
+      <x:c r="N33" s="14"/>
+      <x:c r="O33" s="14"/>
+      <x:c r="P33" s="15"/>
     </x:row>
     <x:row r="34" spans="3:16">
-      <x:c r="C34" s="9"/>
-      <x:c r="D34" s="10"/>
-      <x:c r="E34" s="10"/>
-      <x:c r="F34" s="10"/>
-      <x:c r="G34" s="10"/>
-      <x:c r="H34" s="10"/>
-      <x:c r="I34" s="10"/>
-      <x:c r="J34" s="10"/>
-      <x:c r="K34" s="10"/>
-      <x:c r="L34" s="10"/>
-      <x:c r="M34" s="10"/>
-      <x:c r="N34" s="10"/>
-      <x:c r="O34" s="10"/>
-      <x:c r="P34" s="11"/>
+      <x:c r="C34" s="13"/>
+      <x:c r="D34" s="14"/>
+      <x:c r="E34" s="14"/>
+      <x:c r="F34" s="14"/>
+      <x:c r="G34" s="14"/>
+      <x:c r="H34" s="14"/>
+      <x:c r="I34" s="14"/>
+      <x:c r="J34" s="14"/>
+      <x:c r="K34" s="14"/>
+      <x:c r="L34" s="14"/>
+      <x:c r="M34" s="14"/>
+      <x:c r="N34" s="14"/>
+      <x:c r="O34" s="14"/>
+      <x:c r="P34" s="15"/>
     </x:row>
     <x:row r="35" spans="3:16">
-      <x:c r="C35" s="9"/>
-      <x:c r="D35" s="10"/>
-      <x:c r="E35" s="10"/>
-      <x:c r="F35" s="10"/>
-      <x:c r="G35" s="10"/>
-      <x:c r="H35" s="10"/>
-      <x:c r="I35" s="10"/>
-      <x:c r="J35" s="10"/>
-      <x:c r="K35" s="10"/>
-      <x:c r="L35" s="10"/>
-      <x:c r="M35" s="10"/>
-      <x:c r="N35" s="10"/>
-      <x:c r="O35" s="10"/>
-      <x:c r="P35" s="11"/>
+      <x:c r="C35" s="13"/>
+      <x:c r="D35" s="14"/>
+      <x:c r="E35" s="14"/>
+      <x:c r="F35" s="14"/>
+      <x:c r="G35" s="14"/>
+      <x:c r="H35" s="14"/>
+      <x:c r="I35" s="14"/>
+      <x:c r="J35" s="14"/>
+      <x:c r="K35" s="14"/>
+      <x:c r="L35" s="14"/>
+      <x:c r="M35" s="14"/>
+      <x:c r="N35" s="14"/>
+      <x:c r="O35" s="14"/>
+      <x:c r="P35" s="15"/>
     </x:row>
     <x:row r="36" spans="3:16">
-      <x:c r="C36" s="9"/>
-      <x:c r="D36" s="10"/>
-      <x:c r="E36" s="10"/>
-      <x:c r="F36" s="10"/>
-      <x:c r="G36" s="10"/>
-      <x:c r="H36" s="10"/>
-      <x:c r="I36" s="10"/>
-      <x:c r="J36" s="10"/>
-      <x:c r="K36" s="10"/>
-      <x:c r="L36" s="10"/>
-      <x:c r="M36" s="10"/>
-      <x:c r="N36" s="10"/>
-      <x:c r="O36" s="10"/>
-      <x:c r="P36" s="11"/>
+      <x:c r="C36" s="13"/>
+      <x:c r="D36" s="14"/>
+      <x:c r="E36" s="14"/>
+      <x:c r="F36" s="14"/>
+      <x:c r="G36" s="14"/>
+      <x:c r="H36" s="14"/>
+      <x:c r="I36" s="14"/>
+      <x:c r="J36" s="14"/>
+      <x:c r="K36" s="14"/>
+      <x:c r="L36" s="14"/>
+      <x:c r="M36" s="14"/>
+      <x:c r="N36" s="14"/>
+      <x:c r="O36" s="14"/>
+      <x:c r="P36" s="15"/>
     </x:row>
     <x:row r="37" spans="3:16">
-      <x:c r="C37" s="9"/>
-      <x:c r="D37" s="10"/>
-      <x:c r="E37" s="10"/>
-      <x:c r="F37" s="10"/>
-      <x:c r="G37" s="10"/>
-      <x:c r="H37" s="10"/>
-      <x:c r="I37" s="10"/>
-      <x:c r="J37" s="10"/>
-      <x:c r="K37" s="10"/>
-      <x:c r="L37" s="10"/>
-      <x:c r="M37" s="10"/>
-      <x:c r="N37" s="10"/>
-      <x:c r="O37" s="10"/>
-      <x:c r="P37" s="11"/>
+      <x:c r="C37" s="13"/>
+      <x:c r="D37" s="14"/>
+      <x:c r="E37" s="14"/>
+      <x:c r="F37" s="14"/>
+      <x:c r="G37" s="14"/>
+      <x:c r="H37" s="14"/>
+      <x:c r="I37" s="14"/>
+      <x:c r="J37" s="14"/>
+      <x:c r="K37" s="14"/>
+      <x:c r="L37" s="14"/>
+      <x:c r="M37" s="14"/>
+      <x:c r="N37" s="14"/>
+      <x:c r="O37" s="14"/>
+      <x:c r="P37" s="15"/>
     </x:row>
     <x:row r="38" spans="3:16">
-      <x:c r="C38" s="9"/>
-      <x:c r="D38" s="10"/>
-      <x:c r="E38" s="10"/>
-      <x:c r="F38" s="10"/>
-      <x:c r="G38" s="10"/>
-      <x:c r="H38" s="10"/>
-      <x:c r="I38" s="10"/>
-      <x:c r="J38" s="10"/>
-      <x:c r="K38" s="10"/>
-      <x:c r="L38" s="10"/>
-      <x:c r="M38" s="10"/>
-      <x:c r="N38" s="10"/>
-      <x:c r="O38" s="10"/>
-      <x:c r="P38" s="11"/>
+      <x:c r="C38" s="13"/>
+      <x:c r="D38" s="14"/>
+      <x:c r="E38" s="14"/>
+      <x:c r="F38" s="14"/>
+      <x:c r="G38" s="14"/>
+      <x:c r="H38" s="14"/>
+      <x:c r="I38" s="14"/>
+      <x:c r="J38" s="14"/>
+      <x:c r="K38" s="14"/>
+      <x:c r="L38" s="14"/>
+      <x:c r="M38" s="14"/>
+      <x:c r="N38" s="14"/>
+      <x:c r="O38" s="14"/>
+      <x:c r="P38" s="15"/>
     </x:row>
     <x:row r="39" spans="3:16">
-      <x:c r="C39" s="12"/>
-      <x:c r="D39" s="13"/>
-      <x:c r="E39" s="13"/>
-      <x:c r="F39" s="13"/>
-      <x:c r="G39" s="13"/>
-      <x:c r="H39" s="13"/>
-      <x:c r="I39" s="13"/>
-      <x:c r="J39" s="13"/>
-      <x:c r="K39" s="13"/>
-      <x:c r="L39" s="13"/>
-      <x:c r="M39" s="13"/>
-      <x:c r="N39" s="13"/>
-      <x:c r="O39" s="13"/>
-      <x:c r="P39" s="14"/>
+      <x:c r="C39" s="16"/>
+      <x:c r="D39" s="17"/>
+      <x:c r="E39" s="17"/>
+      <x:c r="F39" s="17"/>
+      <x:c r="G39" s="17"/>
+      <x:c r="H39" s="17"/>
+      <x:c r="I39" s="17"/>
+      <x:c r="J39" s="17"/>
+      <x:c r="K39" s="17"/>
+      <x:c r="L39" s="17"/>
+      <x:c r="M39" s="17"/>
+      <x:c r="N39" s="17"/>
+      <x:c r="O39" s="17"/>
+      <x:c r="P39" s="18"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="1">
     <x:mergeCell ref="C2:P39"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>